<commit_message>
Atualização no Arquivo - 28/12/2020
Adição de novas guias.
</commit_message>
<xml_diff>
--- a/Excel com cara de site_Valmir Santana.xlsx
+++ b/Excel com cara de site_Valmir Santana.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\Documents\Meus projetos\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C43CC1-D953-4A1C-87D3-4B566A1593AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página Inicial" sheetId="1" r:id="rId1"/>
     <sheet name="Histórico Pessoal" sheetId="4" r:id="rId2"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
+    <sheet name="Formação" sheetId="5" r:id="rId3"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId4"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +73,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -89,6 +99,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Fluxograma: Documento 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -167,25 +182,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>114301</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76201</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Fluxograma: Documento 3"/>
+        <xdr:cNvPr id="4" name="Fluxograma: Documento 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4991100" y="38101"/>
-          <a:ext cx="1152525" cy="790574"/>
+          <a:off x="4991101" y="38101"/>
+          <a:ext cx="1181100" cy="790574"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDocument">
           <a:avLst/>
@@ -269,7 +290,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Fluxograma: Documento 4"/>
+        <xdr:cNvPr id="5" name="Fluxograma: Documento 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -359,7 +386,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Fluxograma: Documento 5"/>
+        <xdr:cNvPr id="6" name="Fluxograma: Documento 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -462,7 +495,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Fluxograma: Documento 6"/>
+        <xdr:cNvPr id="7" name="Fluxograma: Documento 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -530,7 +569,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Formação</a:t>
+            <a:t>Formação Educacional</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -544,16 +583,22 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4448175" cy="800099"/>
+    <xdr:ext cx="5705475" cy="800099"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CaixaDeTexto 7"/>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="781050" y="1552575"/>
-          <a:ext cx="4448175" cy="800099"/>
+          <a:ext cx="5705475" cy="800099"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -624,6 +669,112 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Fluxograma: Documento 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341C2A4A-CC3E-484D-A8BD-6D91DFFFF3D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6181725" y="38100"/>
+          <a:ext cx="1181100" cy="790574"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDocument">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F79646">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+            <a:srgbClr val="000000">
+              <a:alpha val="32000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="balanced" dir="t">
+            <a:rot lat="0" lon="0" rev="8700000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="190500" h="38100"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="pt-BR" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Contato</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -644,7 +795,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Fluxograma: Documento 1"/>
+        <xdr:cNvPr id="2" name="Fluxograma: Documento 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -718,13 +875,555 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Gráfico 7" descr="Círculo com seta para a esquerda com preenchimento sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F163AD-12CC-4AB4-ACD5-614021A5FB0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6181726" y="657226"/>
+          <a:ext cx="447674" cy="447674"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Gráfico 12" descr="Círculo com seta para a esquerda com preenchimento sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{245305A3-7959-4DF3-8038-7B00169EB209}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5581650" y="647701"/>
+          <a:ext cx="466724" cy="466724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57152</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Gráfico 14" descr="Início estrutura de tópicos">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6129B6E6-56FA-4DC8-BD82-96415C94DB25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6762752" y="628652"/>
+          <a:ext cx="466724" cy="466724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Gráfico 16" descr="Rolagem estrutura de tópicos">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{287FA0A0-410A-43B0-BA29-E5154914A191}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3019425" y="95250"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Fluxograma: Documento 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{080ECDC6-A42B-4248-A5FC-7217B1939EF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="47625"/>
+          <a:ext cx="1219200" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDocument">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+            <a:srgbClr val="000000">
+              <a:alpha val="32000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="balanced" dir="t">
+            <a:rot lat="0" lon="0" rev="8700000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="190500" h="38100"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Formação</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Educacional</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Gráfico 2" descr="Círculo com seta para a esquerda com preenchimento sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1213411-8439-4CD4-A612-B7C2CAACAEAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6181726" y="657226"/>
+          <a:ext cx="447674" cy="447674"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Gráfico 3" descr="Círculo com seta para a esquerda com preenchimento sólido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA68942E-7FE5-4175-B142-01EA17EA3425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5581650" y="647701"/>
+          <a:ext cx="466724" cy="466724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57152</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Gráfico 4" descr="Início estrutura de tópicos">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D3FDD4-AC68-4A10-93BA-5A1E999811E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6762752" y="628652"/>
+          <a:ext cx="466724" cy="466724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Gráfico 7" descr="Chapéu de formatura com preenchimento sólido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EEB18F7-6569-4ECF-8D5D-0564EBB57568}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057525" y="133350"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -762,9 +1461,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,9 +1496,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,9 +1548,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1007,23 +1740,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="16" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="18" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1040,8 +1771,10 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1058,8 +1791,10 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1076,8 +1811,10 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1094,8 +1831,10 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1112,8 +1851,10 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1124,17 +1865,19 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="17" x14ac:dyDescent="0.25"/>
     <row r="18" x14ac:dyDescent="0.25"/>
     <row r="19" x14ac:dyDescent="0.25"/>
@@ -1148,21 +1891,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Plan2"/>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="16" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="18" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1179,8 +1922,10 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1197,8 +1942,10 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1215,8 +1962,10 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1233,8 +1982,10 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1251,8 +2002,10 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1263,22 +2016,30 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25"/>
-    <row r="17" x14ac:dyDescent="0.25"/>
-    <row r="18" x14ac:dyDescent="0.25"/>
-    <row r="19" x14ac:dyDescent="0.25"/>
-    <row r="20" x14ac:dyDescent="0.25"/>
-    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1287,7 +2048,169 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CF5512-9683-46BA-9891-DAA8F3D6DED7}">
+  <dimension ref="A1:R33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="18" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1299,8 +2222,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1310,4 +2233,172 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CDBB58F8B7769341B20B9BB31225076D" ma:contentTypeVersion="0" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="975d3cc66945b6aa9eab57d4804f7b40">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d058ffe0898091cb30432e4a65399017">
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all/>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3A9C31-5FDB-499F-80AA-AA2E654C3736}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC363F22-0AD8-4FB5-94D1-E3FD9DD465E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9503EF14-3530-499D-AC2B-673866ACDF8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>